<commit_message>
Jan 20 - Updates
</commit_message>
<xml_diff>
--- a/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/CE-Web Catalog .xlsx
+++ b/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/CE-Web Catalog .xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23716"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_3727F2141BCF326DE7A676F1F621E84DE4339CF6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{98F93D73-9496-4D14-8C04-6A131CBAD4E7}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="11_3727F2141BCF326DE7A676F1F621E84DE4339CF6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6885EA47-F22A-4E00-9BB8-7A21C5D3D3E5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="210">
   <si>
     <t>ACQ Sequence</t>
   </si>
@@ -92,6 +92,9 @@
     <t>Fragrance Free</t>
   </si>
   <si>
+    <t> 30D</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kit </t>
   </si>
   <si>
@@ -108,10 +111,38 @@
 I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a full size month supply of Crepe Erase. Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account.</t>
   </si>
   <si>
+    <t>CS2A0464</t>
+  </si>
+  <si>
+    <t>90D</t>
+  </si>
+  <si>
+    <t>RCSA48R</t>
+  </si>
+  <si>
+    <t>"Three months after your first order is shipped, and then every three months thereafter, you will be sent a new full size supply of Crepe Erase®. Each shipment will be charged to the card you provide today, in three monthly payments at the low price of $59.95 plus $3.99 for shipping and handling per month, unless you call to cancel. There is no commitment and no minimum to buy.
+All orders are subject to applicable sales tax."</t>
+  </si>
+  <si>
+    <t>I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase®.  Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account.</t>
+  </si>
+  <si>
     <t>CS2A0459</t>
   </si>
   <si>
     <t>Citrus</t>
+  </si>
+  <si>
+    <t>30D</t>
+  </si>
+  <si>
+    <t>CS2A0465</t>
+  </si>
+  <si>
+    <t>RCSA48V</t>
+  </si>
+  <si>
+    <t>I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a full size month supply of Crepe Erase®.  Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account.</t>
   </si>
   <si>
     <t>CSPG013</t>
@@ -135,7 +166,30 @@
     <t>I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase.  Each full-size shipment will be charged in three payments of $39.95 plus $2.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account.</t>
   </si>
   <si>
+    <t>CS2A0460</t>
+  </si>
+  <si>
+    <t>RCSA48G</t>
+  </si>
+  <si>
+    <t>"Three months after your first order is shipped, and then every three months thereafter, you will be sent a new full size supply of Crepe Erase®. Each shipment will be charged to the card you provide today, in three monthly payments at the low price of $39.95 plus $2.99 for shipping and handling per month, unless you call to cancel. There is no commitment and no minimum to buy.
+All orders are subject to applicable sales tax."</t>
+  </si>
+  <si>
+    <t>I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase®.  Each full-size shipment will be charged in three payments of $39.95 plus $2.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account.</t>
+  </si>
+  <si>
     <t>CS2A0455</t>
+  </si>
+  <si>
+    <t>CS2A0461</t>
+  </si>
+  <si>
+    <t>RCSA48J</t>
+  </si>
+  <si>
+    <t>Three months after your first order is shipped, and then every three months thereafter, you will be sent a new full size supply of Crepe Erase®. Each shipment will be charged to the card you provide today, in three monthly payments at the low price of $39.95 plus $2.99 for shipping and handling per month, unless you call to cancel. There is no commitment and no minimum to buy._x000D_
+All orders are subject to applicable sales tax.</t>
   </si>
   <si>
     <t>CSPG006</t>
@@ -650,7 +704,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -763,6 +817,13 @@
       <color rgb="FF4B4F54"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -893,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -957,17 +1018,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1057,6 +1107,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1277,10 +1350,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1014"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1295,52 +1368,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="30">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="45" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="25"/>
@@ -1355,53 +1428,53 @@
       <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:26" ht="127.5">
-      <c r="A2" s="33">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="30">
+        <v>59.95</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="37">
-        <v>59.95</v>
-      </c>
-      <c r="K2" s="34" t="s">
+      <c r="L2" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="38" t="s">
+      <c r="N2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="44" t="s">
+      <c r="O2" s="31" t="s">
         <v>25</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
@@ -1414,114 +1487,92 @@
       <c r="Y2" s="25"/>
       <c r="Z2" s="25"/>
     </row>
-    <row r="3" spans="1:26" ht="127.5">
-      <c r="A3" s="33">
+    <row r="3" spans="1:26" s="25" customFormat="1" ht="127.5">
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="30">
+        <v>59.95</v>
+      </c>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="127.5">
+      <c r="A4" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="30">
+        <v>59.95</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="37" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="37">
-        <v>59.95</v>
-      </c>
-      <c r="K3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-    </row>
-    <row r="4" spans="1:26" ht="127.5">
-      <c r="A4" s="33">
-        <v>3</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="41">
-        <v>39.950000000000003</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="44" t="s">
-        <v>34</v>
       </c>
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
@@ -1534,114 +1585,92 @@
       <c r="Y4" s="25"/>
       <c r="Z4" s="25"/>
     </row>
-    <row r="5" spans="1:26" ht="127.5">
-      <c r="A5" s="33">
-        <v>4</v>
-      </c>
-      <c r="B5" s="34" t="s">
+    <row r="5" spans="1:26" s="25" customFormat="1" ht="127.5">
+      <c r="A5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="63">
+        <v>59.95</v>
+      </c>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="127.5">
+      <c r="A6" s="26">
+        <v>3</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="34" t="s">
+      <c r="C6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="34" t="s">
+      <c r="F6" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="34">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="K6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="41">
-        <v>39.950000000000003</v>
-      </c>
-      <c r="K5" s="34" t="s">
+      <c r="L6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="M5" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-    </row>
-    <row r="6" spans="1:26" ht="127.5">
-      <c r="A6" s="33">
-        <v>5</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="36">
-        <v>51</v>
-      </c>
-      <c r="K6" s="36">
-        <v>43.35</v>
-      </c>
-      <c r="L6" s="36" t="s">
+      <c r="M6" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="N6" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="34" t="s">
+      <c r="O6" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="P6" s="37" t="s">
         <v>44</v>
-      </c>
-      <c r="P6" s="44" t="s">
-        <v>45</v>
       </c>
       <c r="Q6" s="25"/>
       <c r="R6" s="25"/>
@@ -1654,114 +1683,92 @@
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
     </row>
-    <row r="7" spans="1:26" ht="114.75">
-      <c r="A7" s="33">
-        <v>6</v>
-      </c>
-      <c r="B7" s="53" t="s">
+    <row r="7" spans="1:26" s="25" customFormat="1" ht="127.5">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="34">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="127.5">
+      <c r="A8" s="26">
+        <v>4</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="53" t="s">
+      <c r="C8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="53" t="s">
+      <c r="F8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="53">
-        <v>51</v>
-      </c>
-      <c r="K7" s="53">
-        <v>43.35</v>
-      </c>
-      <c r="L7" s="53" t="s">
+      <c r="G8" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="34">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="M7" s="53" t="s">
+      <c r="N8" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="O7" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-    </row>
-    <row r="8" spans="1:26" ht="127.5">
-      <c r="A8" s="33">
-        <v>7</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="43">
-        <v>69.95</v>
-      </c>
-      <c r="K8" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="O8" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P8" s="44" t="s">
-        <v>56</v>
+      <c r="O8" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>44</v>
       </c>
       <c r="Q8" s="25"/>
       <c r="R8" s="25"/>
@@ -1774,114 +1781,92 @@
       <c r="Y8" s="25"/>
       <c r="Z8" s="25"/>
     </row>
-    <row r="9" spans="1:26" ht="127.5">
-      <c r="A9" s="33">
-        <v>8</v>
-      </c>
-      <c r="B9" s="53" t="s">
+    <row r="9" spans="1:26" s="25" customFormat="1" ht="114.75">
+      <c r="A9" s="26"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="34">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="O9" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="127.5">
+      <c r="A10" s="26">
+        <v>5</v>
+      </c>
+      <c r="B10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="55" t="s">
+      <c r="C10" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="41">
-        <v>69.95</v>
-      </c>
-      <c r="K9" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="45" t="s">
+      <c r="J10" s="29">
+        <v>51</v>
+      </c>
+      <c r="K10" s="29">
+        <v>43.35</v>
+      </c>
+      <c r="L10" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="O9" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P9" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-    </row>
-    <row r="10" spans="1:26" ht="127.5">
-      <c r="A10" s="33">
-        <v>9</v>
-      </c>
-      <c r="B10" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="34" t="s">
+      <c r="M10" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="34" t="s">
+      <c r="N10" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="41">
-        <v>69.95</v>
-      </c>
-      <c r="K10" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="M10" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="45" t="s">
+      <c r="O10" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="O10" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P10" s="44" t="s">
-        <v>56</v>
+      <c r="P10" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="Q10" s="25"/>
       <c r="R10" s="25"/>
@@ -1894,54 +1879,54 @@
       <c r="Y10" s="25"/>
       <c r="Z10" s="25"/>
     </row>
-    <row r="11" spans="1:26" ht="127.5">
-      <c r="A11" s="33">
-        <v>10</v>
-      </c>
-      <c r="B11" s="34" t="s">
+    <row r="11" spans="1:26" ht="114.75">
+      <c r="A11" s="26">
+        <v>6</v>
+      </c>
+      <c r="B11" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="34" t="s">
+      <c r="C11" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="41">
-        <v>69.95</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="45" t="s">
+      <c r="F11" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="46">
+        <v>51</v>
+      </c>
+      <c r="K11" s="46">
+        <v>43.35</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="O11" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="P11" s="44" t="s">
-        <v>56</v>
+      <c r="O11" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="P11" s="37" t="s">
+        <v>66</v>
       </c>
       <c r="Q11" s="25"/>
       <c r="R11" s="25"/>
@@ -1955,53 +1940,53 @@
       <c r="Z11" s="25"/>
     </row>
     <row r="12" spans="1:26" ht="127.5">
-      <c r="A12" s="33">
-        <v>11</v>
-      </c>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="26">
+        <v>7</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="34" t="s">
+      <c r="F12" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="36">
+        <v>69.95</v>
+      </c>
+      <c r="K12" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="34" t="s">
+      <c r="L12" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="41">
-        <v>63</v>
-      </c>
-      <c r="K12" s="41">
-        <v>53.55</v>
-      </c>
-      <c r="L12" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N12" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="O12" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="P12" s="44" t="s">
-        <v>56</v>
+      <c r="N12" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="Q12" s="25"/>
       <c r="R12" s="25"/>
@@ -2015,53 +2000,53 @@
       <c r="Z12" s="25"/>
     </row>
     <row r="13" spans="1:26" ht="127.5">
-      <c r="A13" s="33">
-        <v>12</v>
-      </c>
-      <c r="B13" s="34" t="s">
+      <c r="A13" s="26">
+        <v>8</v>
+      </c>
+      <c r="B13" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="34" t="s">
+      <c r="F13" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="34">
+        <v>69.95</v>
+      </c>
+      <c r="K13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="L13" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" s="41">
-        <v>72</v>
-      </c>
-      <c r="K13" s="41">
-        <v>61.2</v>
-      </c>
-      <c r="L13" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M13" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N13" s="45" t="s">
+      <c r="P13" s="37" t="s">
         <v>73</v>
-      </c>
-      <c r="O13" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="P13" s="34" t="s">
-        <v>75</v>
       </c>
       <c r="Q13" s="25"/>
       <c r="R13" s="25"/>
@@ -2075,53 +2060,53 @@
       <c r="Z13" s="25"/>
     </row>
     <row r="14" spans="1:26" ht="127.5">
-      <c r="A14" s="33">
-        <v>13</v>
-      </c>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="26">
+        <v>9</v>
+      </c>
+      <c r="B14" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="E14" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="H14" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="34">
+        <v>69.95</v>
+      </c>
+      <c r="K14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="L14" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="41">
-        <v>25</v>
-      </c>
-      <c r="K14" s="41">
-        <v>21.25</v>
-      </c>
-      <c r="L14" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N14" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="O14" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="P14" s="34" t="s">
-        <v>81</v>
+      <c r="O14" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="25"/>
@@ -2134,54 +2119,54 @@
       <c r="Y14" s="25"/>
       <c r="Z14" s="25"/>
     </row>
-    <row r="15" spans="1:26" ht="114.75">
-      <c r="A15" s="33">
-        <v>14</v>
-      </c>
-      <c r="B15" s="53" t="s">
+    <row r="15" spans="1:26" ht="127.5">
+      <c r="A15" s="26">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="34" t="s">
+      <c r="C15" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="34" t="s">
+      <c r="F15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="34">
+        <v>69.95</v>
+      </c>
+      <c r="K15" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="41">
-        <v>25</v>
-      </c>
-      <c r="K15" s="41">
-        <v>21.25</v>
-      </c>
-      <c r="L15" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N15" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="O15" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="P15" s="34" t="s">
+      <c r="L15" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="38" t="s">
         <v>81</v>
+      </c>
+      <c r="O15" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="25"/>
@@ -2194,54 +2179,54 @@
       <c r="Y15" s="25"/>
       <c r="Z15" s="25"/>
     </row>
-    <row r="16" spans="1:26" ht="114.75">
-      <c r="A16" s="33">
-        <v>15</v>
-      </c>
-      <c r="B16" s="53" t="s">
+    <row r="16" spans="1:26" ht="127.5">
+      <c r="A16" s="26">
+        <v>11</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="34" t="s">
+      <c r="C16" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="41">
-        <v>25</v>
-      </c>
-      <c r="K16" s="41">
-        <v>21.25</v>
-      </c>
-      <c r="L16" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M16" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="34" t="s">
+      <c r="I16" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="34">
+        <v>63</v>
+      </c>
+      <c r="K16" s="34">
+        <v>53.55</v>
+      </c>
+      <c r="L16" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="O16" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="P16" s="34" t="s">
-        <v>81</v>
+      <c r="N16" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="O16" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="P16" s="37" t="s">
+        <v>73</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="25"/>
@@ -2254,54 +2239,54 @@
       <c r="Y16" s="25"/>
       <c r="Z16" s="25"/>
     </row>
-    <row r="17" spans="1:26" ht="114.75">
-      <c r="A17" s="33">
+    <row r="17" spans="1:26" ht="127.5">
+      <c r="A17" s="26">
+        <v>12</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="C17" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="34" t="s">
+      <c r="D17" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="34" t="s">
+      <c r="F17" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="41">
-        <v>25</v>
-      </c>
-      <c r="K17" s="41">
-        <v>21.25</v>
-      </c>
-      <c r="L17" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="O17" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="P17" s="34" t="s">
-        <v>81</v>
+      <c r="H17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="34">
+        <v>72</v>
+      </c>
+      <c r="K17" s="34">
+        <v>61.2</v>
+      </c>
+      <c r="L17" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="O17" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="P17" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="25"/>
@@ -2314,54 +2299,54 @@
       <c r="Y17" s="25"/>
       <c r="Z17" s="25"/>
     </row>
-    <row r="18" spans="1:26" ht="114.75">
-      <c r="A18" s="33">
-        <v>17</v>
-      </c>
-      <c r="B18" s="36" t="s">
+    <row r="18" spans="1:26" ht="127.5">
+      <c r="A18" s="26">
+        <v>13</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="34" t="s">
+      <c r="C18" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="34" t="s">
+      <c r="F18" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J18" s="41">
-        <v>22</v>
-      </c>
-      <c r="K18" s="41">
-        <v>18.7</v>
-      </c>
-      <c r="L18" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M18" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N18" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="O18" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="P18" s="34" t="s">
-        <v>93</v>
+      <c r="I18" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="34">
+        <v>25</v>
+      </c>
+      <c r="K18" s="34">
+        <v>21.25</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="O18" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="P18" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="25"/>
@@ -2375,53 +2360,53 @@
       <c r="Z18" s="25"/>
     </row>
     <row r="19" spans="1:26" ht="114.75">
-      <c r="A19" s="33">
-        <v>18</v>
-      </c>
-      <c r="B19" s="53" t="s">
+      <c r="A19" s="26">
+        <v>14</v>
+      </c>
+      <c r="B19" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="34" t="s">
+      <c r="C19" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="34" t="s">
+      <c r="F19" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J19" s="41">
-        <v>22</v>
-      </c>
-      <c r="K19" s="41">
-        <v>18.7</v>
-      </c>
-      <c r="L19" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="O19" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="P19" s="34" t="s">
-        <v>93</v>
+      <c r="I19" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="34">
+        <v>25</v>
+      </c>
+      <c r="K19" s="34">
+        <v>21.25</v>
+      </c>
+      <c r="L19" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="O19" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="P19" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="25"/>
@@ -2435,53 +2420,53 @@
       <c r="Z19" s="25"/>
     </row>
     <row r="20" spans="1:26" ht="114.75">
-      <c r="A20" s="33">
-        <v>19</v>
-      </c>
-      <c r="B20" s="53" t="s">
+      <c r="A20" s="26">
+        <v>15</v>
+      </c>
+      <c r="B20" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="34" t="s">
+      <c r="C20" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="59" t="s">
+      <c r="F20" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="34">
+        <v>25</v>
+      </c>
+      <c r="K20" s="34">
+        <v>21.25</v>
+      </c>
+      <c r="L20" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M20" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N20" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="O20" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="H20" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J20" s="41">
-        <v>22</v>
-      </c>
-      <c r="K20" s="41">
-        <v>18.7</v>
-      </c>
-      <c r="L20" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M20" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N20" s="58" t="s">
+      <c r="P20" s="27" t="s">
         <v>98</v>
-      </c>
-      <c r="O20" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="P20" s="34" t="s">
-        <v>93</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="25"/>
@@ -2495,53 +2480,53 @@
       <c r="Z20" s="25"/>
     </row>
     <row r="21" spans="1:26" ht="114.75">
-      <c r="A21" s="33">
-        <v>20</v>
-      </c>
-      <c r="B21" s="53" t="s">
+      <c r="A21" s="26">
         <v>16</v>
       </c>
-      <c r="C21" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="34" t="s">
+      <c r="B21" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="34" t="s">
+      <c r="C21" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J21" s="41">
-        <v>22</v>
-      </c>
-      <c r="K21" s="41">
-        <v>18.7</v>
-      </c>
-      <c r="L21" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M21" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N21" s="58" t="s">
-        <v>100</v>
-      </c>
-      <c r="O21" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="P21" s="34" t="s">
-        <v>93</v>
+      <c r="F21" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="34">
+        <v>25</v>
+      </c>
+      <c r="K21" s="34">
+        <v>21.25</v>
+      </c>
+      <c r="L21" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N21" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="O21" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="P21" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
@@ -2555,53 +2540,53 @@
       <c r="Z21" s="25"/>
     </row>
     <row r="22" spans="1:26" ht="114.75">
-      <c r="A22" s="33">
-        <v>21</v>
-      </c>
-      <c r="B22" s="53" t="s">
+      <c r="A22" s="26">
+        <v>17</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="34" t="s">
+      <c r="C22" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="H22" s="34" t="s">
+      <c r="F22" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J22" s="41">
+      <c r="I22" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="34">
         <v>22</v>
       </c>
-      <c r="K22" s="41">
+      <c r="K22" s="34">
         <v>18.7</v>
       </c>
-      <c r="L22" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M22" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N22" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="O22" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="P22" s="34" t="s">
-        <v>93</v>
+      <c r="L22" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="N22" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="O22" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="P22" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="25"/>
@@ -2615,53 +2600,53 @@
       <c r="Z22" s="25"/>
     </row>
     <row r="23" spans="1:26" ht="114.75">
-      <c r="A23" s="33">
+      <c r="A23" s="26">
+        <v>18</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="34">
         <v>22</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>104</v>
-      </c>
-      <c r="H23" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="41">
-        <v>22</v>
-      </c>
-      <c r="K23" s="41">
+      <c r="K23" s="34">
         <v>18.7</v>
       </c>
-      <c r="L23" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M23" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="N23" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="O23" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="P23" s="34" t="s">
-        <v>93</v>
+      <c r="L23" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="N23" s="51" t="s">
+        <v>112</v>
+      </c>
+      <c r="O23" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P23" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="25"/>
@@ -2675,53 +2660,53 @@
       <c r="Z23" s="25"/>
     </row>
     <row r="24" spans="1:26" ht="114.75">
-      <c r="A24" s="33">
-        <v>23</v>
-      </c>
-      <c r="B24" s="36" t="s">
+      <c r="A24" s="26">
+        <v>19</v>
+      </c>
+      <c r="B24" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D24" s="34" t="s">
+      <c r="C24" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="G24" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J24" s="41">
-        <v>44</v>
-      </c>
-      <c r="K24" s="41">
-        <v>37.4</v>
-      </c>
-      <c r="L24" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M24" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N24" s="61" t="s">
+      <c r="I24" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="34">
+        <v>22</v>
+      </c>
+      <c r="K24" s="34">
+        <v>18.7</v>
+      </c>
+      <c r="L24" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="N24" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="O24" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="O24" s="46" t="s">
+      <c r="P24" s="27" t="s">
         <v>110</v>
-      </c>
-      <c r="P24" s="34" t="s">
-        <v>111</v>
       </c>
       <c r="Q24" s="25"/>
       <c r="R24" s="25"/>
@@ -2735,53 +2720,53 @@
       <c r="Z24" s="25"/>
     </row>
     <row r="25" spans="1:26" ht="114.75">
-      <c r="A25" s="33">
-        <v>24</v>
-      </c>
-      <c r="B25" s="34" t="s">
+      <c r="A25" s="26">
+        <v>20</v>
+      </c>
+      <c r="B25" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="34" t="s">
+      <c r="C25" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="34" t="s">
+      <c r="F25" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="41">
-        <v>44</v>
-      </c>
-      <c r="K25" s="41">
-        <v>37.4</v>
-      </c>
-      <c r="L25" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M25" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N25" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="O25" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="P25" s="34" t="s">
-        <v>111</v>
+      <c r="I25" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="34">
+        <v>22</v>
+      </c>
+      <c r="K25" s="34">
+        <v>18.7</v>
+      </c>
+      <c r="L25" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="N25" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="O25" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P25" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
@@ -2795,53 +2780,53 @@
       <c r="Z25" s="25"/>
     </row>
     <row r="26" spans="1:26" ht="114.75">
-      <c r="A26" s="33">
-        <v>25</v>
-      </c>
-      <c r="B26" s="36" t="s">
+      <c r="A26" s="26">
+        <v>21</v>
+      </c>
+      <c r="B26" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="E26" s="34" t="s">
+      <c r="C26" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="34" t="s">
+      <c r="F26" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" s="41">
-        <v>44</v>
-      </c>
-      <c r="K26" s="41">
-        <v>37.4</v>
-      </c>
-      <c r="L26" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M26" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N26" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="O26" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="P26" s="34" t="s">
-        <v>120</v>
+      <c r="I26" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" s="34">
+        <v>22</v>
+      </c>
+      <c r="K26" s="34">
+        <v>18.7</v>
+      </c>
+      <c r="L26" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="N26" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="O26" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P26" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="Q26" s="25"/>
       <c r="R26" s="25"/>
@@ -2855,53 +2840,53 @@
       <c r="Z26" s="25"/>
     </row>
     <row r="27" spans="1:26" ht="114.75">
-      <c r="A27" s="33">
-        <v>26</v>
-      </c>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="26">
+        <v>22</v>
+      </c>
+      <c r="B27" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="40" t="s">
-        <v>115</v>
-      </c>
-      <c r="D27" s="34" t="s">
+      <c r="C27" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="H27" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="G27" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J27" s="41">
-        <v>44</v>
-      </c>
-      <c r="K27" s="41">
-        <v>37.4</v>
-      </c>
-      <c r="L27" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M27" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N27" s="58" t="s">
+      <c r="I27" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="34">
+        <v>22</v>
+      </c>
+      <c r="K27" s="34">
+        <v>18.7</v>
+      </c>
+      <c r="L27" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="N27" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="O27" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="P27" s="45" t="s">
-        <v>120</v>
+      <c r="O27" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="P27" s="27" t="s">
+        <v>110</v>
       </c>
       <c r="Q27" s="25"/>
       <c r="R27" s="25"/>
@@ -2915,53 +2900,53 @@
       <c r="Z27" s="25"/>
     </row>
     <row r="28" spans="1:26" ht="114.75">
-      <c r="A28" s="33">
-        <v>27</v>
-      </c>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="26">
+        <v>23</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" s="34" t="s">
+      <c r="F28" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F28" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J28" s="41">
-        <v>75</v>
-      </c>
-      <c r="K28" s="41">
-        <v>63.75</v>
-      </c>
-      <c r="L28" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M28" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N28" s="61" t="s">
-        <v>125</v>
-      </c>
-      <c r="O28" s="48" t="s">
+      <c r="I28" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J28" s="34">
+        <v>44</v>
+      </c>
+      <c r="K28" s="34">
+        <v>37.4</v>
+      </c>
+      <c r="L28" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="P28" s="44" t="s">
+      <c r="O28" s="39" t="s">
         <v>127</v>
+      </c>
+      <c r="P28" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="Q28" s="25"/>
       <c r="R28" s="25"/>
@@ -2975,53 +2960,53 @@
       <c r="Z28" s="25"/>
     </row>
     <row r="29" spans="1:26" ht="114.75">
-      <c r="A29" s="33">
-        <v>28</v>
-      </c>
-      <c r="B29" s="34" t="s">
+      <c r="A29" s="26">
+        <v>24</v>
+      </c>
+      <c r="B29" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="F29" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" s="34">
+        <v>44</v>
+      </c>
+      <c r="K29" s="34">
+        <v>37.4</v>
+      </c>
+      <c r="L29" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N29" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="O29" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="P29" s="27" t="s">
         <v>128</v>
-      </c>
-      <c r="E29" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J29" s="41">
-        <v>38</v>
-      </c>
-      <c r="K29" s="41">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="L29" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M29" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="N29" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="O29" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="P29" s="44" t="s">
-        <v>133</v>
       </c>
       <c r="Q29" s="25"/>
       <c r="R29" s="25"/>
@@ -3034,54 +3019,54 @@
       <c r="Y29" s="25"/>
       <c r="Z29" s="25"/>
     </row>
-    <row r="30" spans="1:26" ht="127.5">
-      <c r="A30" s="33">
-        <v>29</v>
-      </c>
-      <c r="B30" s="34" t="s">
+    <row r="30" spans="1:26" ht="114.75">
+      <c r="A30" s="26">
+        <v>25</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="F30" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="G30" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="45" t="s">
+      <c r="I30" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="34">
+        <v>44</v>
+      </c>
+      <c r="K30" s="34">
+        <v>37.4</v>
+      </c>
+      <c r="L30" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="G30" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J30" s="41">
-        <v>54</v>
-      </c>
-      <c r="K30" s="41">
-        <v>45.9</v>
-      </c>
-      <c r="L30" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N30" s="45" t="s">
+      <c r="O30" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="O30" s="38" t="s">
+      <c r="P30" s="27" t="s">
         <v>137</v>
-      </c>
-      <c r="P30" s="44" t="s">
-        <v>138</v>
       </c>
       <c r="Q30" s="25"/>
       <c r="R30" s="25"/>
@@ -3094,54 +3079,54 @@
       <c r="Y30" s="25"/>
       <c r="Z30" s="25"/>
     </row>
-    <row r="31" spans="1:26" ht="127.5">
-      <c r="A31" s="33">
-        <v>30</v>
-      </c>
-      <c r="B31" s="34" t="s">
+    <row r="31" spans="1:26" ht="114.75">
+      <c r="A31" s="26">
+        <v>26</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="39" t="s">
+      <c r="F31" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="34">
+        <v>44</v>
+      </c>
+      <c r="K31" s="34">
+        <v>37.4</v>
+      </c>
+      <c r="L31" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J31" s="41">
-        <v>22</v>
-      </c>
-      <c r="K31" s="41">
-        <v>18.7</v>
-      </c>
-      <c r="L31" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M31" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N31" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="O31" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="P31" s="44" t="s">
-        <v>143</v>
+      <c r="O31" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="P31" s="38" t="s">
+        <v>137</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31" s="25"/>
@@ -3154,54 +3139,54 @@
       <c r="Y31" s="25"/>
       <c r="Z31" s="25"/>
     </row>
-    <row r="32" spans="1:26" ht="127.5">
-      <c r="A32" s="33">
-        <v>31</v>
-      </c>
-      <c r="B32" s="34" t="s">
+    <row r="32" spans="1:26" ht="114.75">
+      <c r="A32" s="26">
+        <v>27</v>
+      </c>
+      <c r="B32" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" s="34">
+        <v>75</v>
+      </c>
+      <c r="K32" s="34">
+        <v>63.75</v>
+      </c>
+      <c r="L32" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M32" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="O32" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="P32" s="37" t="s">
         <v>144</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="G32" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="J32" s="41">
-        <v>30</v>
-      </c>
-      <c r="K32" s="41">
-        <v>25.5</v>
-      </c>
-      <c r="L32" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="M32" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="N32" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="O32" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="P32" s="44" t="s">
-        <v>148</v>
       </c>
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
@@ -3214,54 +3199,54 @@
       <c r="Y32" s="25"/>
       <c r="Z32" s="25"/>
     </row>
-    <row r="33" spans="1:26" ht="127.5">
-      <c r="A33" s="33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="34" t="s">
+    <row r="33" spans="1:26" ht="114.75">
+      <c r="A33" s="26">
+        <v>28</v>
+      </c>
+      <c r="B33" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" s="34">
+        <v>38</v>
+      </c>
+      <c r="K33" s="34">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="L33" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M33" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="N33" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="O33" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="E33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="35" t="s">
+      <c r="P33" s="37" t="s">
         <v>150</v>
-      </c>
-      <c r="G33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="J33" s="41">
-        <v>59.95</v>
-      </c>
-      <c r="K33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L33" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="M33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="O33" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="P33" s="44" t="s">
-        <v>154</v>
       </c>
       <c r="Q33" s="25"/>
       <c r="R33" s="25"/>
@@ -3275,53 +3260,53 @@
       <c r="Z33" s="25"/>
     </row>
     <row r="34" spans="1:26" ht="127.5">
-      <c r="A34" s="33">
-        <v>33</v>
-      </c>
-      <c r="B34" s="34" t="s">
+      <c r="A34" s="26">
+        <v>29</v>
+      </c>
+      <c r="B34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" s="34">
+        <v>54</v>
+      </c>
+      <c r="K34" s="34">
+        <v>45.9</v>
+      </c>
+      <c r="L34" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N34" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="O34" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="P34" s="37" t="s">
         <v>155</v>
-      </c>
-      <c r="E34" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="J34" s="41">
-        <v>39.950000000000003</v>
-      </c>
-      <c r="K34" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="L34" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="M34" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="N34" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="O34" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="P34" s="44" t="s">
-        <v>159</v>
       </c>
       <c r="Q34" s="25"/>
       <c r="R34" s="25"/>
@@ -3334,54 +3319,54 @@
       <c r="Y34" s="25"/>
       <c r="Z34" s="25"/>
     </row>
-    <row r="35" spans="1:26" ht="12.75">
-      <c r="A35" s="62" t="s">
+    <row r="35" spans="1:26" ht="127.5">
+      <c r="A35" s="26">
+        <v>30</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="G35" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J35" s="34">
+        <v>22</v>
+      </c>
+      <c r="K35" s="34">
+        <v>18.7</v>
+      </c>
+      <c r="L35" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M35" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N35" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="O35" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="P35" s="37" t="s">
         <v>160</v>
-      </c>
-      <c r="B35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="K35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="L35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="M35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="N35" s="60" t="s">
-        <v>16</v>
-      </c>
-      <c r="O35" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="P35" s="62" t="s">
-        <v>16</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="25"/>
@@ -3394,23 +3379,55 @@
       <c r="Y35" s="25"/>
       <c r="Z35" s="25"/>
     </row>
-    <row r="36" spans="1:26" ht="12.75">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="2"/>
+    <row r="36" spans="1:26" ht="127.5">
+      <c r="A36" s="26">
+        <v>31</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="34">
+        <v>30</v>
+      </c>
+      <c r="K36" s="34">
+        <v>25.5</v>
+      </c>
+      <c r="L36" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N36" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="O36" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="P36" s="37" t="s">
+        <v>165</v>
+      </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
@@ -3422,23 +3439,55 @@
       <c r="Y36" s="25"/>
       <c r="Z36" s="25"/>
     </row>
-    <row r="37" spans="1:26" ht="12.75">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="2"/>
+    <row r="37" spans="1:26" ht="127.5">
+      <c r="A37" s="26">
+        <v>32</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J37" s="34">
+        <v>59.95</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="M37" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="O37" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="P37" s="37" t="s">
+        <v>171</v>
+      </c>
       <c r="Q37" s="25"/>
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
@@ -3450,23 +3499,55 @@
       <c r="Y37" s="25"/>
       <c r="Z37" s="25"/>
     </row>
-    <row r="38" spans="1:26" ht="12.75">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="2"/>
+    <row r="38" spans="1:26" ht="127.5">
+      <c r="A38" s="26">
+        <v>33</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J38" s="34">
+        <v>39.950000000000003</v>
+      </c>
+      <c r="K38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="M38" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="O38" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="P38" s="37" t="s">
+        <v>176</v>
+      </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="25"/>
       <c r="S38" s="25"/>
@@ -3479,22 +3560,54 @@
       <c r="Z38" s="25"/>
     </row>
     <row r="39" spans="1:26" ht="12.75">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="2"/>
+      <c r="A39" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="P39" s="55" t="s">
+        <v>16</v>
+      </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
@@ -3522,7 +3635,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
+      <c r="P40" s="2"/>
       <c r="Q40" s="25"/>
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
@@ -3634,7 +3747,7 @@
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="2"/>
+      <c r="P44" s="1"/>
       <c r="Q44" s="25"/>
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
@@ -3997,7 +4110,7 @@
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
+      <c r="O57" s="1"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="25"/>
       <c r="R57" s="25"/>
@@ -4025,7 +4138,7 @@
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
+      <c r="O58" s="1"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="25"/>
       <c r="R58" s="25"/>
@@ -4053,7 +4166,7 @@
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
+      <c r="O59" s="1"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="25"/>
       <c r="R59" s="25"/>
@@ -4081,7 +4194,7 @@
       <c r="L60" s="2"/>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
+      <c r="O60" s="1"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="25"/>
       <c r="R60" s="25"/>
@@ -30806,36 +30919,148 @@
       <c r="Y1014" s="25"/>
       <c r="Z1014" s="25"/>
     </row>
+    <row r="1015" spans="1:26" ht="12.75">
+      <c r="A1015" s="2"/>
+      <c r="B1015" s="2"/>
+      <c r="C1015" s="2"/>
+      <c r="D1015" s="2"/>
+      <c r="E1015" s="2"/>
+      <c r="F1015" s="2"/>
+      <c r="G1015" s="2"/>
+      <c r="H1015" s="2"/>
+      <c r="I1015" s="2"/>
+      <c r="J1015" s="2"/>
+      <c r="K1015" s="2"/>
+      <c r="L1015" s="2"/>
+      <c r="M1015" s="2"/>
+      <c r="N1015" s="2"/>
+      <c r="O1015" s="2"/>
+      <c r="P1015" s="2"/>
+      <c r="Q1015" s="25"/>
+      <c r="R1015" s="25"/>
+      <c r="S1015" s="25"/>
+      <c r="T1015" s="25"/>
+      <c r="U1015" s="25"/>
+      <c r="V1015" s="25"/>
+      <c r="W1015" s="25"/>
+      <c r="X1015" s="25"/>
+      <c r="Y1015" s="25"/>
+      <c r="Z1015" s="25"/>
+    </row>
+    <row r="1016" spans="1:26" ht="12.75">
+      <c r="A1016" s="2"/>
+      <c r="B1016" s="2"/>
+      <c r="C1016" s="2"/>
+      <c r="D1016" s="2"/>
+      <c r="E1016" s="2"/>
+      <c r="F1016" s="2"/>
+      <c r="G1016" s="2"/>
+      <c r="H1016" s="2"/>
+      <c r="I1016" s="2"/>
+      <c r="J1016" s="2"/>
+      <c r="K1016" s="2"/>
+      <c r="L1016" s="2"/>
+      <c r="M1016" s="2"/>
+      <c r="N1016" s="2"/>
+      <c r="O1016" s="2"/>
+      <c r="P1016" s="2"/>
+      <c r="Q1016" s="25"/>
+      <c r="R1016" s="25"/>
+      <c r="S1016" s="25"/>
+      <c r="T1016" s="25"/>
+      <c r="U1016" s="25"/>
+      <c r="V1016" s="25"/>
+      <c r="W1016" s="25"/>
+      <c r="X1016" s="25"/>
+      <c r="Y1016" s="25"/>
+      <c r="Z1016" s="25"/>
+    </row>
+    <row r="1017" spans="1:26" ht="12.75">
+      <c r="A1017" s="2"/>
+      <c r="B1017" s="2"/>
+      <c r="C1017" s="2"/>
+      <c r="D1017" s="2"/>
+      <c r="E1017" s="2"/>
+      <c r="F1017" s="2"/>
+      <c r="G1017" s="2"/>
+      <c r="H1017" s="2"/>
+      <c r="I1017" s="2"/>
+      <c r="J1017" s="2"/>
+      <c r="K1017" s="2"/>
+      <c r="L1017" s="2"/>
+      <c r="M1017" s="2"/>
+      <c r="N1017" s="2"/>
+      <c r="O1017" s="2"/>
+      <c r="P1017" s="2"/>
+      <c r="Q1017" s="25"/>
+      <c r="R1017" s="25"/>
+      <c r="S1017" s="25"/>
+      <c r="T1017" s="25"/>
+      <c r="U1017" s="25"/>
+      <c r="V1017" s="25"/>
+      <c r="W1017" s="25"/>
+      <c r="X1017" s="25"/>
+      <c r="Y1017" s="25"/>
+      <c r="Z1017" s="25"/>
+    </row>
+    <row r="1018" spans="1:26" ht="12.75">
+      <c r="A1018" s="2"/>
+      <c r="B1018" s="2"/>
+      <c r="C1018" s="2"/>
+      <c r="D1018" s="2"/>
+      <c r="E1018" s="2"/>
+      <c r="F1018" s="2"/>
+      <c r="G1018" s="2"/>
+      <c r="H1018" s="2"/>
+      <c r="I1018" s="2"/>
+      <c r="J1018" s="2"/>
+      <c r="K1018" s="2"/>
+      <c r="L1018" s="2"/>
+      <c r="M1018" s="2"/>
+      <c r="N1018" s="2"/>
+      <c r="O1018" s="2"/>
+      <c r="P1018" s="2"/>
+      <c r="Q1018" s="25"/>
+      <c r="R1018" s="25"/>
+      <c r="S1018" s="25"/>
+      <c r="T1018" s="25"/>
+      <c r="U1018" s="25"/>
+      <c r="V1018" s="25"/>
+      <c r="W1018" s="25"/>
+      <c r="X1018" s="25"/>
+      <c r="Y1018" s="25"/>
+      <c r="Z1018" s="25"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="_x000a_I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a full size month supply of Crepe Erase. Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{EED8F3C4-1046-4DE7-8F42-4A999A748211}"/>
-    <hyperlink ref="P3" r:id="rId2" display="_x000a_I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a full size month supply of Crepe Erase. Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{7698F08C-F966-49E4-8677-E0EC572EB175}"/>
-    <hyperlink ref="P4" r:id="rId3" display="I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase.  Each full-size shipment will be charged in three payments of $39.95 plus $2.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{A3116318-20F8-4B78-BEFC-93192FB99527}"/>
-    <hyperlink ref="P5" r:id="rId4" display="I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase.  Each full-size shipment will be charged in three payments of $39.95 plus $2.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{3F0DAD38-D9D7-4B06-AD0E-E8CD1248B040}"/>
-    <hyperlink ref="P6" r:id="rId5" display="_x000a_I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Body Smoothing Pre-Treatment. Each shipment will be charged in one payment of $43.35 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{5D7B3AB6-2899-40FE-A090-22CB6D1D80FD}"/>
-    <hyperlink ref="P7" r:id="rId6" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Body Smoothing Pre-Treatment. Each shipment will be charged in one payment of $43.35 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{DB39AC91-03E8-4E26-9DFE-7F8E2EA2DAEC}"/>
-    <hyperlink ref="P8" r:id="rId7" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{EFF9F149-3D93-42B6-BDC8-49CB2B67B206}"/>
-    <hyperlink ref="P9" r:id="rId8" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{39C96049-5B76-4AA4-AC80-6329E70347D5}"/>
-    <hyperlink ref="P10" r:id="rId9" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{30CBD294-3BA9-42EF-87F3-9E98D72C3FEB}"/>
-    <hyperlink ref="P11" r:id="rId10" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{32103C0E-2A3B-4F28-906F-F4DE28E10C95}"/>
-    <hyperlink ref="F13" r:id="rId11" xr:uid="{9788B78F-55F8-4E16-8A82-D38A1C250238}"/>
-    <hyperlink ref="P13" r:id="rId12" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Toning and Tightening Body Serum. Each shipment will be charged in one payment of $61.20 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{EBA2477F-DB47-43E8-81AB-1C5771AFAA04}"/>
-    <hyperlink ref="P14" r:id="rId13" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Body Hydrating Body Toning Mist. Each shipment will be charged in one payment of $21.25 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{C9865B45-597A-43CD-8475-28681AF0658C}"/>
-    <hyperlink ref="P18" r:id="rId14" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{7EFF2CDD-E372-4DD0-8D5D-1559209D812B}"/>
-    <hyperlink ref="P19" r:id="rId15" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{273C79CA-3A01-43E6-8D11-C5D7D21255A3}"/>
-    <hyperlink ref="P20" r:id="rId16" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{D5CD33BC-46CD-42A3-B638-059F049E5D5C}"/>
-    <hyperlink ref="P21" r:id="rId17" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{A51124D9-AD10-4544-8B99-E80C7F45F10E}"/>
-    <hyperlink ref="P22" r:id="rId18" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{B014FE79-102C-4222-83E8-B56BD21D554E}"/>
-    <hyperlink ref="P23" r:id="rId19" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{435D13A3-5FB9-4D48-81F9-55FCF40BAC70}"/>
-    <hyperlink ref="F26" r:id="rId20" xr:uid="{F2D62773-DFFA-4953-9407-C516FE4A3CDC}"/>
-    <hyperlink ref="P26" r:id="rId21" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Restorative Facial Treatment. Each shipment will be charged in one payment of $37.40 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{202CAA70-7800-4457-B375-B7D6023E77DD}"/>
-    <hyperlink ref="F27" r:id="rId22" xr:uid="{A30651FB-9F6B-4121-BAA2-6842BEBCA697}"/>
-    <hyperlink ref="P28" r:id="rId23" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Flaw-Fix™ Eye Cream. Each shipment will be charged in one payment of $63.75 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{D1BE8443-698F-4898-881C-147B942CFD45}"/>
-    <hyperlink ref="P29" r:id="rId24" display="I understand that one month after my first order is shipped, and then every month thereafter, I will be sent a new full size supply of Crepe Erase Line Smoothing Capsules. Each shipment will be charged in one payment of $32.30 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{6DCAD8ED-7322-49F4-986A-C47CE0330E67}"/>
-    <hyperlink ref="F30" r:id="rId25" xr:uid="{7C0C6F90-9ECD-407D-97DE-35091D10C7C8}"/>
-    <hyperlink ref="P31" r:id="rId26" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Flaw-Fix™ Intensive Lip Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{11298519-0819-49B2-BFA9-20F8B4086A1C}"/>
-    <hyperlink ref="P33" r:id="rId27" display="I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase®. Each shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{443E3DB1-192A-4D97-AF89-1E018D5DD024}"/>
-    <hyperlink ref="P27" r:id="rId28" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Restorative Facial Treatment. Each shipment will be charged in one payment of $37.40 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{5B446DC7-D5A0-4AF8-9CE4-B58A14E51B92}"/>
+    <hyperlink ref="P31" r:id="rId1" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Restorative Facial Treatment. Each shipment will be charged in one payment of $37.40 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{5B446DC7-D5A0-4AF8-9CE4-B58A14E51B92}"/>
+    <hyperlink ref="P37" r:id="rId2" display="I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase®. Each shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{443E3DB1-192A-4D97-AF89-1E018D5DD024}"/>
+    <hyperlink ref="P35" r:id="rId3" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Flaw-Fix™ Intensive Lip Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{11298519-0819-49B2-BFA9-20F8B4086A1C}"/>
+    <hyperlink ref="F34" r:id="rId4" xr:uid="{7C0C6F90-9ECD-407D-97DE-35091D10C7C8}"/>
+    <hyperlink ref="P33" r:id="rId5" display="I understand that one month after my first order is shipped, and then every month thereafter, I will be sent a new full size supply of Crepe Erase Line Smoothing Capsules. Each shipment will be charged in one payment of $32.30 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{6DCAD8ED-7322-49F4-986A-C47CE0330E67}"/>
+    <hyperlink ref="P32" r:id="rId6" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Flaw-Fix™ Eye Cream. Each shipment will be charged in one payment of $63.75 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{D1BE8443-698F-4898-881C-147B942CFD45}"/>
+    <hyperlink ref="F31" r:id="rId7" xr:uid="{A30651FB-9F6B-4121-BAA2-6842BEBCA697}"/>
+    <hyperlink ref="P30" r:id="rId8" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Restorative Facial Treatment. Each shipment will be charged in one payment of $37.40 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{202CAA70-7800-4457-B375-B7D6023E77DD}"/>
+    <hyperlink ref="F30" r:id="rId9" xr:uid="{F2D62773-DFFA-4953-9407-C516FE4A3CDC}"/>
+    <hyperlink ref="P27" r:id="rId10" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{435D13A3-5FB9-4D48-81F9-55FCF40BAC70}"/>
+    <hyperlink ref="P26" r:id="rId11" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{B014FE79-102C-4222-83E8-B56BD21D554E}"/>
+    <hyperlink ref="P25" r:id="rId12" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{A51124D9-AD10-4544-8B99-E80C7F45F10E}"/>
+    <hyperlink ref="P24" r:id="rId13" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{D5CD33BC-46CD-42A3-B638-059F049E5D5C}"/>
+    <hyperlink ref="P23" r:id="rId14" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{273C79CA-3A01-43E6-8D11-C5D7D21255A3}"/>
+    <hyperlink ref="P22" r:id="rId15" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Anti-Aging Hand Repair Treatment. Each shipment will be charged in one payment of $18.70 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{7EFF2CDD-E372-4DD0-8D5D-1559209D812B}"/>
+    <hyperlink ref="P18" r:id="rId16" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Body Hydrating Body Toning Mist. Each shipment will be charged in one payment of $21.25 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{C9865B45-597A-43CD-8475-28681AF0658C}"/>
+    <hyperlink ref="P17" r:id="rId17" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase® Toning and Tightening Body Serum. Each shipment will be charged in one payment of $61.20 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{EBA2477F-DB47-43E8-81AB-1C5771AFAA04}"/>
+    <hyperlink ref="F17" r:id="rId18" xr:uid="{9788B78F-55F8-4E16-8A82-D38A1C250238}"/>
+    <hyperlink ref="P15" r:id="rId19" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{32103C0E-2A3B-4F28-906F-F4DE28E10C95}"/>
+    <hyperlink ref="P14" r:id="rId20" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{30CBD294-3BA9-42EF-87F3-9E98D72C3FEB}"/>
+    <hyperlink ref="P13" r:id="rId21" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{39C96049-5B76-4AA4-AC80-6329E70347D5}"/>
+    <hyperlink ref="P12" r:id="rId22" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Advanced Body Repair Treatment. Each shipment will be charged in one payment of $69.95 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{EFF9F149-3D93-42B6-BDC8-49CB2B67B206}"/>
+    <hyperlink ref="P11" r:id="rId23" display="I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Body Smoothing Pre-Treatment. Each shipment will be charged in one payment of $43.35 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{DB39AC91-03E8-4E26-9DFE-7F8E2EA2DAEC}"/>
+    <hyperlink ref="P10" r:id="rId24" display="_x000a_I understand that three months after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase Body Smoothing Pre-Treatment. Each shipment will be charged in one payment of $43.35 plus $5.99 for shipping and handling. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{5D7B3AB6-2899-40FE-A090-22CB6D1D80FD}"/>
+    <hyperlink ref="P8" r:id="rId25" display="I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase.  Each full-size shipment will be charged in three payments of $39.95 plus $2.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{3F0DAD38-D9D7-4B06-AD0E-E8CD1248B040}"/>
+    <hyperlink ref="P6" r:id="rId26" display="I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a new full size supply of Crepe Erase.  Each full-size shipment will be charged in three payments of $39.95 plus $2.99 for shipping and handling per month.  I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{A3116318-20F8-4B78-BEFC-93192FB99527}"/>
+    <hyperlink ref="P4" r:id="rId27" display="_x000a_I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a full size month supply of Crepe Erase. Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{7698F08C-F966-49E4-8677-E0EC572EB175}"/>
+    <hyperlink ref="P2" r:id="rId28" display="_x000a_I understand that one month after my first order is shipped, and then every three months thereafter, I will be sent a full size month supply of Crepe Erase. Each full-size shipment will be charged in three payments of $59.95 plus $3.99 for shipping and handling per month. I understand there is no minimum to buy, and I can easily customize or cancel this program just by visiting crepeerase.com/account." xr:uid="{EED8F3C4-1046-4DE7-8F42-4A999A748211}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
@@ -30886,53 +31111,53 @@
         <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="Q1" s="25"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="30">
+      <c r="A2" s="59">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="26" t="s">
-        <v>36</v>
+      <c r="B2" s="56"/>
+      <c r="C2" s="60" t="s">
+        <v>53</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="H2" s="19">
         <v>51</v>
@@ -30964,20 +31189,20 @@
       <c r="Q2" s="25"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="4" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="H3" s="19">
         <v>51</v>
@@ -31009,24 +31234,24 @@
       <c r="Q3" s="11"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="30">
+      <c r="A4" s="59">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="26" t="s">
-        <v>50</v>
+      <c r="B4" s="56"/>
+      <c r="C4" s="60" t="s">
+        <v>67</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="H4" s="19">
         <v>69.95</v>
@@ -31050,17 +31275,17 @@
       <c r="Q4" s="25"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="21" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="19">
@@ -31093,17 +31318,17 @@
       <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="18" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="19">
@@ -31136,17 +31361,17 @@
       <c r="Q6" s="25"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
       <c r="D7" s="4" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="19">
@@ -31185,14 +31410,14 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="18" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="H8" s="19">
         <v>63</v>
@@ -31214,10 +31439,10 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="18" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -31241,21 +31466,21 @@
       <c r="Q9" s="25"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="30">
+      <c r="A10" s="59">
         <v>5</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29" t="s">
-        <v>76</v>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56" t="s">
+        <v>93</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="19">
@@ -31278,17 +31503,17 @@
       <c r="Q10" s="25"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="18" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="19">
@@ -31319,17 +31544,17 @@
       <c r="Q11" s="25"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="18" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="19">
@@ -31360,17 +31585,17 @@
       <c r="Q12" s="25"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="21" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="19">
@@ -31401,18 +31626,18 @@
       <c r="Q13" s="25"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="30">
+      <c r="A14" s="59">
         <v>6</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29" t="s">
-        <v>88</v>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56" t="s">
+        <v>105</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>20</v>
@@ -31446,17 +31671,17 @@
       <c r="Q14" s="25"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="18" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="19">
@@ -31487,17 +31712,17 @@
       <c r="Q15" s="25"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="21" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="19">
@@ -31528,17 +31753,17 @@
       <c r="Q16" s="25"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="18" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="19">
@@ -31568,17 +31793,17 @@
       </c>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="18" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="19">
@@ -31608,17 +31833,17 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="58"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="18" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="19">
@@ -31648,21 +31873,21 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="30">
+      <c r="A20" s="59">
         <v>7</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29" t="s">
-        <v>106</v>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56" t="s">
+        <v>123</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="19">
@@ -31694,17 +31919,17 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="18" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="19">
@@ -31736,21 +31961,21 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="30">
+      <c r="A22" s="59">
         <v>8</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="31" t="s">
-        <v>115</v>
+      <c r="B22" s="56"/>
+      <c r="C22" s="61" t="s">
+        <v>132</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="19">
@@ -31782,17 +32007,17 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="32"/>
+      <c r="A23" s="58"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="62"/>
       <c r="D23" s="3" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="19">
@@ -31830,10 +32055,10 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="18" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -31870,10 +32095,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="1"/>
       <c r="D25" s="18" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -31896,10 +32121,10 @@
       <c r="B26" s="3"/>
       <c r="C26" s="1"/>
       <c r="D26" s="15" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -31936,10 +32161,10 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="20" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -31976,10 +32201,10 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="18" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -32016,10 +32241,10 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="18" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -32042,10 +32267,10 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="18" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -32099,24 +32324,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="A4:A7"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C14:C19"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -32129,6 +32354,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C47EEB8100460B478BDC3BCCBE3D5051" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="829e995fc61fbfa25718206016b29da6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2" xmlns:ns3="3e63a3be-2d53-41f2-914e-dd0efc332534" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3545440ad2b936a9d10385f8b267d779" ns2:_="" ns3:_="">
     <xsd:import namespace="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2"/>
@@ -32293,23 +32533,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{719136BB-1F5B-45E6-86D2-22A09E3FE4F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA921101-522F-453B-9EC3-3F7A00A0E732}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32317,5 +32542,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA921101-522F-453B-9EC3-3F7A00A0E732}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{719136BB-1F5B-45E6-86D2-22A09E3FE4F6}"/>
 </file>
</xml_diff>